<commit_message>
Replaced all files with updated IndicPhotoOCR version
</commit_message>
<xml_diff>
--- a/Evaluation/Evaluations.xlsx
+++ b/Evaluation/Evaluations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a469ffe22e27418b/Naisa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\IndicPhotoOcr\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{DD176BD7-143D-405F-B45C-B8E6D61072F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF547B4-1986-43D9-8657-E1112355F69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1221739F-9329-402D-9F59-DC6951D23502}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{1221739F-9329-402D-9F59-DC6951D23502}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,163 +63,163 @@
     <t xml:space="preserve">Bengoli </t>
   </si>
   <si>
-    <t>img2</t>
-  </si>
-  <si>
-    <t>img3</t>
-  </si>
-  <si>
     <t>Correctly Recognized</t>
   </si>
   <si>
-    <t>img4</t>
-  </si>
-  <si>
-    <t>img8</t>
-  </si>
-  <si>
-    <t>img9</t>
-  </si>
-  <si>
-    <t>img10</t>
-  </si>
-  <si>
-    <t>img11</t>
-  </si>
-  <si>
-    <t>img12</t>
-  </si>
-  <si>
-    <t>img13</t>
-  </si>
-  <si>
-    <t>img14</t>
-  </si>
-  <si>
-    <t>img15</t>
-  </si>
-  <si>
-    <t>img16</t>
-  </si>
-  <si>
-    <t>Img5</t>
-  </si>
-  <si>
-    <t>Img6</t>
-  </si>
-  <si>
-    <t>Img7</t>
-  </si>
-  <si>
-    <t>img17</t>
-  </si>
-  <si>
-    <t>img18</t>
-  </si>
-  <si>
-    <t>img19</t>
-  </si>
-  <si>
-    <t>img20</t>
-  </si>
-  <si>
-    <t>img21</t>
-  </si>
-  <si>
-    <t>img22</t>
-  </si>
-  <si>
-    <t>img23</t>
-  </si>
-  <si>
-    <t>img24</t>
-  </si>
-  <si>
-    <t>img25</t>
-  </si>
-  <si>
-    <t>img26</t>
-  </si>
-  <si>
-    <t>img27</t>
-  </si>
-  <si>
-    <t>img28</t>
-  </si>
-  <si>
-    <t>img29</t>
-  </si>
-  <si>
-    <t>img30</t>
-  </si>
-  <si>
-    <t>img31</t>
-  </si>
-  <si>
-    <t>img32</t>
-  </si>
-  <si>
-    <t>img33</t>
-  </si>
-  <si>
-    <t>img34</t>
-  </si>
-  <si>
-    <t>img35</t>
-  </si>
-  <si>
-    <t>img36</t>
-  </si>
-  <si>
-    <t>img37</t>
-  </si>
-  <si>
-    <t>img38</t>
-  </si>
-  <si>
-    <t>img39</t>
-  </si>
-  <si>
-    <t>img40</t>
-  </si>
-  <si>
-    <t>img41</t>
-  </si>
-  <si>
-    <t>img42</t>
-  </si>
-  <si>
-    <t>img43</t>
-  </si>
-  <si>
-    <t>img44</t>
-  </si>
-  <si>
-    <t>img45</t>
-  </si>
-  <si>
-    <t>img46</t>
-  </si>
-  <si>
-    <t>img47</t>
-  </si>
-  <si>
-    <t>img48</t>
-  </si>
-  <si>
-    <t>img49</t>
-  </si>
-  <si>
-    <t>img50</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>img1</t>
-  </si>
-  <si>
-    <t>Word Recognition rate=0.756637</t>
+    <t>Word Recognition rate=0.757056</t>
+  </si>
+  <si>
+    <t>ce65d6fd-IMG_20250525_064605</t>
+  </si>
+  <si>
+    <t>fbf718a9-IMG_20250525_064639</t>
+  </si>
+  <si>
+    <t>42536b22-IMG_20250525_195135</t>
+  </si>
+  <si>
+    <t>b1c2b1b0-IMG_20250525_195316</t>
+  </si>
+  <si>
+    <t>70dbecaa-IMG_20250525_195350</t>
+  </si>
+  <si>
+    <t>095ac2dc-IMG_20250525_202538</t>
+  </si>
+  <si>
+    <t>fe223f4d-IMG_20250525_202612</t>
+  </si>
+  <si>
+    <t>de96e70c-IMG_20250525_202638</t>
+  </si>
+  <si>
+    <t>4b7b017b-IMG_20250525_202657</t>
+  </si>
+  <si>
+    <t>5d183998-IMG_20250525_202719</t>
+  </si>
+  <si>
+    <t>1db1d7a9-IMG_20250525_202820</t>
+  </si>
+  <si>
+    <t>97bd0c79-IMG_20250525_202853</t>
+  </si>
+  <si>
+    <t>e450f7bc-IMG_20250525_202929</t>
+  </si>
+  <si>
+    <t>d0df8a04-IMG_20250525_203004</t>
+  </si>
+  <si>
+    <t>8c477614-IMG_20250525_203022</t>
+  </si>
+  <si>
+    <t>91b7342b-IMG_20250525_203046</t>
+  </si>
+  <si>
+    <t>6c493789-IMG_20250528_212325</t>
+  </si>
+  <si>
+    <t>0951b8c6-IMG_20250528_212407</t>
+  </si>
+  <si>
+    <t>d72ae2f6-IMG_20250528_212431</t>
+  </si>
+  <si>
+    <t>bd0cae1f-IMG_20250601_130047</t>
+  </si>
+  <si>
+    <t>929908c8-IMG_20250601_130137</t>
+  </si>
+  <si>
+    <t>26063cb2-IMG_20250601_130309</t>
+  </si>
+  <si>
+    <t>9518d017-IMG_20250601_130324</t>
+  </si>
+  <si>
+    <t>ef682f83-IMG_20250601_130420</t>
+  </si>
+  <si>
+    <t>a00f9bf4-IMG_20250601_130449</t>
+  </si>
+  <si>
+    <t>7c32edcc-IMG_20250601_130510</t>
+  </si>
+  <si>
+    <t>bfa9423f-IMG_20250601_130535</t>
+  </si>
+  <si>
+    <t>98ea8985-IMG_20250601_130553</t>
+  </si>
+  <si>
+    <t>f6f0a47e-IMG_20250601_130622</t>
+  </si>
+  <si>
+    <t>6b995825-IMG_20250601_130638</t>
+  </si>
+  <si>
+    <t>171b0dce-IMG_20250601_130655</t>
+  </si>
+  <si>
+    <t>bbb9963c-IMG_20250601_130720</t>
+  </si>
+  <si>
+    <t>51e8f8d6-IMG_20250601_130744</t>
+  </si>
+  <si>
+    <t>183badc6-IMG_20250601_130805</t>
+  </si>
+  <si>
+    <t>396eea1c-IMG_20250601_130824</t>
+  </si>
+  <si>
+    <t>df2390c1-IMG_20250601_130940</t>
+  </si>
+  <si>
+    <t>5e2af95a-IMG_20250601_131004</t>
+  </si>
+  <si>
+    <t>0809e706-IMG_20250601_131026</t>
+  </si>
+  <si>
+    <t>ec522c72-IMG_20250601_131038</t>
+  </si>
+  <si>
+    <t>a569ade5-IMG_20250601_131058</t>
+  </si>
+  <si>
+    <t>3157e8ff-IMG_20250601_131123</t>
+  </si>
+  <si>
+    <t>c37e43b7-IMG_20250601_131203</t>
+  </si>
+  <si>
+    <t>395af569-IMG_20250601_131237</t>
+  </si>
+  <si>
+    <t>3acdfa00-IMG_20250601_131334</t>
+  </si>
+  <si>
+    <t>69ea5ac2-IMG_20250601_133910</t>
+  </si>
+  <si>
+    <t>5a278303-IMG20250525084754</t>
+  </si>
+  <si>
+    <t>ff6c56f3-IMG20250609053807</t>
+  </si>
+  <si>
+    <t>699fbbc0-IMG_20250601_130245</t>
+  </si>
+  <si>
+    <t>47b6167b-IMG_20250601_130847</t>
+  </si>
+  <si>
+    <t>83487cd5-IMG_20250601_131135</t>
   </si>
 </sst>
 </file>
@@ -269,9 +269,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -287,10 +288,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -592,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8033B83E-C3C8-440C-9E42-1B1B51DB15DA}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +606,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -641,7 +638,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>18</v>
@@ -671,7 +668,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -700,7 +697,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>16</v>
@@ -730,87 +727,109 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <f>22/28</f>
+        <v>0.7857142857142857</v>
       </c>
       <c r="F5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <f>22/28</f>
-        <v>0.7857142857142857</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <f>18/20</f>
+        <v>0.9</v>
+      </c>
+      <c r="F7">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="C8">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="D8">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E8">
-        <f>18/20</f>
-        <v>0.9</v>
+        <f>46/58</f>
+        <v>0.7931034482758621</v>
       </c>
       <c r="F8">
         <v>11</v>
@@ -819,189 +838,189 @@
         <v>11</v>
       </c>
       <c r="H8">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="I8">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B9">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C9">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="D9">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E9">
-        <f>46/58</f>
-        <v>0.7931034482758621</v>
+        <f>33/35</f>
+        <v>0.94285714285714284</v>
       </c>
       <c r="F9">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G9">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H9">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="I9">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B10">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E10">
-        <f>33/35</f>
-        <v>0.94285714285714284</v>
+        <f>25/34</f>
+        <v>0.73529411764705888</v>
       </c>
       <c r="F10">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G10">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H10">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="I10">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C11">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D11">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E11">
-        <f>25/34</f>
-        <v>0.73529411764705888</v>
+        <f>39/47</f>
+        <v>0.82978723404255317</v>
       </c>
       <c r="F11">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G11">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H11">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="I11">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <f>25/29</f>
+        <v>0.86206896551724133</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
         <v>16</v>
       </c>
-      <c r="B12">
+      <c r="H12">
+        <v>9</v>
+      </c>
+      <c r="I12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>45</v>
+      </c>
+      <c r="C13">
+        <v>39</v>
+      </c>
+      <c r="D13">
+        <v>35</v>
+      </c>
+      <c r="E13">
+        <f>35/45</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>40</v>
+      </c>
+      <c r="I13">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="C12">
+      <c r="B14">
         <v>22</v>
       </c>
-      <c r="D12">
+      <c r="C14">
+        <v>22</v>
+      </c>
+      <c r="D14">
         <v>18</v>
       </c>
-      <c r="E12">
+      <c r="E14">
         <f>18/22</f>
         <v>0.81818181818181823</v>
       </c>
-      <c r="F12">
+      <c r="F14">
         <v>22</v>
       </c>
-      <c r="G12">
+      <c r="G14">
         <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13">
-        <v>29</v>
-      </c>
-      <c r="C13">
-        <v>27</v>
-      </c>
-      <c r="D13">
-        <v>25</v>
-      </c>
-      <c r="E13">
-        <f>25/29</f>
-        <v>0.86206896551724133</v>
-      </c>
-      <c r="F13">
-        <v>20</v>
-      </c>
-      <c r="G13">
-        <v>16</v>
-      </c>
-      <c r="H13">
-        <v>9</v>
-      </c>
-      <c r="I13">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <v>45</v>
-      </c>
-      <c r="C14">
-        <v>39</v>
-      </c>
-      <c r="D14">
-        <v>35</v>
-      </c>
-      <c r="E14">
-        <f>35/45</f>
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="F14">
-        <v>5</v>
-      </c>
-      <c r="G14">
-        <v>4</v>
-      </c>
-      <c r="H14">
-        <v>40</v>
-      </c>
-      <c r="I14">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>39</v>
@@ -1025,7 +1044,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>24</v>
@@ -1055,7 +1074,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>31</v>
@@ -1085,67 +1104,86 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>46</v>
+      </c>
+      <c r="C18">
+        <v>41</v>
+      </c>
+      <c r="D18">
+        <v>35</v>
+      </c>
+      <c r="E18">
+        <f>35/46</f>
+        <v>0.76086956521739135</v>
+      </c>
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18">
+        <v>11</v>
+      </c>
+      <c r="H18">
+        <v>30</v>
+      </c>
+      <c r="I18">
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B19">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C19">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D19">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E19">
-        <f>35/46</f>
-        <v>0.76086956521739135</v>
+        <f>22/39</f>
+        <v>0.5641025641025641</v>
       </c>
       <c r="F19">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G19">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H19">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I19">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>28</v>
+      </c>
+      <c r="C20">
         <v>27</v>
       </c>
-      <c r="B20">
-        <v>39</v>
-      </c>
-      <c r="C20">
-        <v>25</v>
-      </c>
       <c r="D20">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E20">
-        <f>22/39</f>
-        <v>0.5641025641025641</v>
+        <f>27/28</f>
+        <v>0.9642857142857143</v>
       </c>
       <c r="F20">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G20">
-        <v>8</v>
-      </c>
-      <c r="H20">
-        <v>29</v>
-      </c>
-      <c r="I20">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1153,28 +1191,28 @@
         <v>28</v>
       </c>
       <c r="B21">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C21">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D21">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E21">
-        <f>27/28</f>
-        <v>0.9642857142857143</v>
+        <f>17/23</f>
+        <v>0.73913043478260865</v>
       </c>
       <c r="F21">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G21">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B22">
         <v>12</v>
@@ -1203,7 +1241,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B23">
         <v>15</v>
@@ -1233,7 +1271,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>7</v>
@@ -1262,7 +1300,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B25">
         <v>7</v>
@@ -1291,7 +1329,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>31</v>
@@ -1321,7 +1359,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -1351,7 +1389,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B28">
         <v>16</v>
@@ -1375,7 +1413,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B29">
         <v>14</v>
@@ -1405,7 +1443,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B30">
         <v>4</v>
@@ -1429,7 +1467,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B31">
         <v>28</v>
@@ -1459,7 +1497,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B32">
         <v>17</v>
@@ -1489,7 +1527,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B33">
         <v>9</v>
@@ -1513,166 +1551,191 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="B34">
+        <v>15</v>
+      </c>
+      <c r="C34">
+        <v>11</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <f>10/15</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F34">
+        <v>15</v>
+      </c>
+      <c r="G34">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B35">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C35">
+        <v>13</v>
+      </c>
+      <c r="D35">
+        <v>9</v>
+      </c>
+      <c r="E35">
+        <f>9/13</f>
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="F35">
         <v>11</v>
       </c>
-      <c r="D35">
-        <v>10</v>
-      </c>
-      <c r="E35">
-        <f>10/15</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="F35">
-        <v>15</v>
-      </c>
       <c r="G35">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B36">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C36">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D36">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E36">
-        <f>9/13</f>
-        <v>0.69230769230769229</v>
+        <v>1</v>
       </c>
       <c r="F36">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G36">
-        <v>9</v>
-      </c>
-      <c r="H36">
-        <v>2</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B37">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C37">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D37">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>15</v>
-      </c>
-      <c r="G37">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38">
-        <v>12</v>
-      </c>
-      <c r="C38">
-        <v>10</v>
-      </c>
-      <c r="D38">
-        <v>10</v>
-      </c>
-      <c r="E38">
         <f>10/12</f>
         <v>0.83333333333333337</v>
       </c>
+      <c r="F37">
+        <v>12</v>
+      </c>
+      <c r="G37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>7</v>
+      </c>
+      <c r="E38">
+        <f>7/8</f>
+        <v>0.875</v>
+      </c>
       <c r="F38">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G38">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
+      <c r="I38">
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B39">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C39">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D39">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E39">
-        <f>7/8</f>
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G39">
-        <v>4</v>
-      </c>
-      <c r="H39">
-        <v>4</v>
-      </c>
-      <c r="I39">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D40">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <f>3/8</f>
+        <v>0.375</v>
       </c>
       <c r="F40">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G40">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>6</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B41">
         <v>5</v>
@@ -1701,124 +1764,143 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="B42">
+        <v>23</v>
+      </c>
+      <c r="C42">
+        <v>16</v>
+      </c>
+      <c r="D42">
+        <v>12</v>
+      </c>
+      <c r="E42">
+        <f>12/23</f>
+        <v>0.52173913043478259</v>
+      </c>
+      <c r="F42">
+        <v>23</v>
+      </c>
+      <c r="G42">
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B43">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C43">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D43">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E43">
-        <f>12/23</f>
-        <v>0.52173913043478259</v>
+        <v>1</v>
       </c>
       <c r="F43">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="G43">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>18</v>
+      </c>
+      <c r="I43">
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B44">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C44">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D44">
         <v>19</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <f>19/22</f>
+        <v>0.86363636363636365</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H44">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I44">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B45">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C45">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E45">
-        <f>19/22</f>
-        <v>0.86363636363636365</v>
+        <v>1</v>
       </c>
       <c r="F45">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G45">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H45">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="I45">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <f>8/10</f>
+        <v>0.8</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G46">
-        <v>1</v>
-      </c>
-      <c r="H46">
-        <v>1</v>
-      </c>
-      <c r="I46">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B47">
         <v>20</v>
@@ -1848,7 +1930,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -1884,7 +1966,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B49">
         <v>9</v>
@@ -1914,7 +1996,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B50">
         <v>12</v>
@@ -1944,7 +2026,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -1973,35 +2055,35 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="B53" s="1">
         <f>SUM(B2:B52)</f>
-        <v>904</v>
+        <v>992</v>
       </c>
       <c r="C53" s="1">
         <f>SUM(C2:C52)</f>
-        <v>787</v>
+        <v>865</v>
       </c>
       <c r="D53" s="1">
         <f>SUM(D2:D52)</f>
-        <v>684</v>
+        <v>751</v>
       </c>
       <c r="F53" s="1">
         <f>SUM(F2:F52)</f>
-        <v>462</v>
+        <v>521</v>
       </c>
       <c r="G53" s="1">
         <f>SUM(G2:G52)</f>
-        <v>356</v>
+        <v>404</v>
       </c>
       <c r="H53" s="1">
         <f>SUM(H2:H52)</f>
-        <v>440</v>
+        <v>469</v>
       </c>
       <c r="I53" s="1">
         <f>SUM(I2:I52)</f>
-        <v>328</v>
+        <v>347</v>
       </c>
       <c r="J53">
         <v>1</v>
@@ -2018,7 +2100,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>

</xml_diff>